<commit_message>
CS61C Proj03: Task 6 R-type Instructions
</commit_message>
<xml_diff>
--- a/[61C FA22] Project 3B ROM Control Logic.xlsx
+++ b/[61C FA22] Project 3B ROM Control Logic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/misaka/Downloads/Course/System/CS61C/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/misaka/Downloads/Course/System/CS61C/proj/proj03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECB5AFC-5586-674D-AF34-41D7108A4DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE03B8D-C327-E64A-B8BB-8C8A181AC519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control Logic for ROM" sheetId="1" r:id="rId1"/>
@@ -727,19 +727,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -752,6 +743,15 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -986,7 +986,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1003,20 +1003,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="33" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="35" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="32" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="29"/>
@@ -1025,11 +1025,11 @@
       <c r="L1" s="29"/>
       <c r="M1" s="29"/>
       <c r="N1" s="29"/>
-      <c r="O1" s="34"/>
+      <c r="O1" s="31"/>
       <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="33" t="s">
         <v>5</v>
       </c>
       <c r="R1" s="29"/>
@@ -1047,7 +1047,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="34" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="29"/>
@@ -1056,7 +1056,7 @@
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
-      <c r="O2" s="34"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -1182,10 +1182,10 @@
       <c r="A5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="35" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="17" t="s">
@@ -2098,10 +2098,10 @@
       <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="37" t="s">
         <v>60</v>
       </c>
       <c r="D17" s="17" t="s">
@@ -2277,7 +2277,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="29"/>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="37" t="s">
         <v>64</v>
       </c>
       <c r="D20" s="17" t="s">
@@ -2876,10 +2876,10 @@
       <c r="A28" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="37" t="s">
         <v>79</v>
       </c>
       <c r="D28" s="17" t="s">
@@ -3054,10 +3054,10 @@
       <c r="A31" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="37" t="s">
         <v>84</v>
       </c>
       <c r="D31" s="17" t="s">
@@ -3406,7 +3406,7 @@
       <c r="A37" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="36" t="s">
         <v>91</v>
       </c>
       <c r="C37" s="25" t="s">
@@ -3644,12 +3644,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="H2:O2"/>
     <mergeCell ref="C5:C16"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="B37:B38"/>
@@ -3660,6 +3654,12 @@
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="C31:C36"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="H2:O2"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="A1:A2">

</xml_diff>

<commit_message>
CS61C Proj03: ROM Control Logic
</commit_message>
<xml_diff>
--- a/[61C FA22] Project 3B ROM Control Logic.xlsx
+++ b/[61C FA22] Project 3B ROM Control Logic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/misaka/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A1E757-905F-7E4D-8A40-4B0A7093EAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA50913-DC03-D348-BC8F-1D70E31846D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,6 +45,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>This is the value that will be passed into the ROM</t>
@@ -58,6 +59,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>This is the value that will be outputted from the ROM. It's all the control signals concatenated together.</t>
@@ -71,6 +73,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>This is the value that will be outputted from the ROM. It's all the control signals concatenated together.</t>
@@ -84,7 +87,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <scheme val="minor"/>
+            <family val="2"/>
           </rPr>
           <t>This value is provided as an example. Based on your design for the immediate generator, you may need to modify this value to generate the correct immediate value</t>
         </r>
@@ -123,7 +126,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <scheme val="minor"/>
+            <family val="2"/>
           </rPr>
           <t>This value is provided as an example. Based on your design for the B MUX, you may need to modify this value to generate the correct immediate value</t>
         </r>
@@ -136,7 +139,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <scheme val="minor"/>
+            <family val="2"/>
           </rPr>
           <t>This value is provided as an example. Based on your design for the Writeback MUX, you may need to modify this value to generate the correct immediate value</t>
         </r>
@@ -147,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="118">
   <si>
     <t>MAKE A COPY OF THIS SHEET</t>
   </si>
@@ -480,13 +483,34 @@
   </si>
   <si>
     <t>0111</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -582,6 +606,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -720,6 +751,7 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -746,7 +778,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -977,10 +1008,10 @@
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J33" sqref="J33"/>
+      <selection pane="bottomRight" activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -997,60 +1028,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="30"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="31"/>
       <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="Q1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="28"/>
+      <c r="A2" s="29"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="30"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -1176,10 +1207,10 @@
       <c r="A5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="35" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="17" t="s">
@@ -1196,28 +1227,28 @@
         <f t="shared" ref="G5:G40" si="0">V5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="37" t="s">
+      <c r="H5" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="J5" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K5" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M5" s="37" t="s">
+      <c r="J5" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="O5" s="37" t="s">
+      <c r="N5" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" s="27" t="s">
         <v>69</v>
       </c>
       <c r="P5" s="11" t="str">
@@ -1256,8 +1287,8 @@
       <c r="A6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="17" t="s">
         <v>36</v>
       </c>
@@ -1272,25 +1303,25 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J6" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K6" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L6" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M6" s="37" t="s">
+      <c r="J6" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O6" s="19" t="s">
@@ -1332,8 +1363,8 @@
       <c r="A7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="17" t="s">
         <v>36</v>
       </c>
@@ -1348,25 +1379,25 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I7" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J7" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K7" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L7" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M7" s="37" t="s">
+      <c r="J7" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="N7" s="37" t="s">
+      <c r="N7" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O7" s="19" t="s">
@@ -1408,8 +1439,8 @@
       <c r="A8" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="17" t="s">
         <v>43</v>
       </c>
@@ -1424,25 +1455,25 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K8" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M8" s="37" t="s">
+      <c r="J8" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="N8" s="37" t="s">
+      <c r="N8" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O8" s="19" t="s">
@@ -1484,8 +1515,8 @@
       <c r="A9" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="20" t="s">
         <v>43</v>
       </c>
@@ -1500,25 +1531,25 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K9" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M9" s="37" t="s">
+      <c r="J9" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O9" s="19" t="s">
@@ -1560,8 +1591,8 @@
       <c r="A10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="17" t="s">
         <v>46</v>
       </c>
@@ -1576,25 +1607,25 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J10" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K10" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L10" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M10" s="37" t="s">
+      <c r="J10" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="N10" s="37" t="s">
+      <c r="N10" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O10" s="19" t="s">
@@ -1636,8 +1667,8 @@
       <c r="A11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="17" t="s">
         <v>48</v>
       </c>
@@ -1652,25 +1683,25 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K11" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L11" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M11" s="37" t="s">
+      <c r="J11" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="N11" s="37" t="s">
+      <c r="N11" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O11" s="19" t="s">
@@ -1712,8 +1743,8 @@
       <c r="A12" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="17" t="s">
         <v>50</v>
       </c>
@@ -1728,25 +1759,25 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J12" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K12" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L12" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M12" s="37" t="s">
+      <c r="J12" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="N12" s="37" t="s">
+      <c r="N12" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O12" s="19" t="s">
@@ -1788,8 +1819,8 @@
       <c r="A13" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
       <c r="D13" s="17" t="s">
         <v>52</v>
       </c>
@@ -1804,25 +1835,25 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H13" s="37" t="s">
+      <c r="H13" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J13" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K13" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L13" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M13" s="37" t="s">
+      <c r="J13" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="N13" s="37" t="s">
+      <c r="N13" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O13" s="19" t="s">
@@ -1864,8 +1895,8 @@
       <c r="A14" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="17" t="s">
         <v>52</v>
       </c>
@@ -1880,25 +1911,25 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J14" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K14" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L14" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M14" s="37" t="s">
+      <c r="J14" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="N14" s="37" t="s">
+      <c r="N14" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O14" s="19" t="s">
@@ -1940,8 +1971,8 @@
       <c r="A15" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="17" t="s">
         <v>55</v>
       </c>
@@ -1956,25 +1987,25 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H15" s="37" t="s">
+      <c r="H15" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K15" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L15" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M15" s="37" t="s">
+      <c r="J15" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="37" t="s">
+      <c r="N15" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O15" s="19" t="s">
@@ -2016,8 +2047,8 @@
       <c r="A16" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
       <c r="D16" s="17" t="s">
         <v>57</v>
       </c>
@@ -2032,25 +2063,25 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="H16" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I16" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J16" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K16" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L16" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M16" s="37" t="s">
+      <c r="J16" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M16" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="N16" s="37" t="s">
+      <c r="N16" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O16" s="19" t="s">
@@ -2092,10 +2123,10 @@
       <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="37" t="s">
         <v>60</v>
       </c>
       <c r="D17" s="17" t="s">
@@ -2110,37 +2141,53 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
+      <c r="H17" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M17" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N17" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="O17" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P17" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0841</v>
       </c>
       <c r="Q17" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100001000001</v>
       </c>
       <c r="R17" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000001</v>
       </c>
       <c r="S17" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T17" s="12" t="str">
         <f t="shared" ref="T17:U17" si="18">BIN2HEX(R17,2)</f>
-        <v>00</v>
+        <v>41</v>
       </c>
       <c r="U17" s="13" t="str">
         <f t="shared" si="18"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V17" s="12">
         <v>12</v>
@@ -2150,12 +2197,12 @@
         <v>001100</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="20" t="s">
         <v>43</v>
       </c>
@@ -2168,37 +2215,53 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
+      <c r="H18" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M18" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N18" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="O18" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P18" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0841</v>
       </c>
       <c r="Q18" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100001000001</v>
       </c>
       <c r="R18" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000001</v>
       </c>
       <c r="S18" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T18" s="12" t="str">
         <f t="shared" ref="T18:U18" si="19">BIN2HEX(R18,2)</f>
-        <v>00</v>
+        <v>41</v>
       </c>
       <c r="U18" s="13" t="str">
         <f t="shared" si="19"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V18" s="12">
         <v>13</v>
@@ -2208,12 +2271,12 @@
         <v>001101</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="17" t="s">
         <v>48</v>
       </c>
@@ -2226,37 +2289,53 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
+      <c r="H19" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M19" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N19" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="O19" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P19" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0841</v>
       </c>
       <c r="Q19" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100001000001</v>
       </c>
       <c r="R19" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000001</v>
       </c>
       <c r="S19" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T19" s="12" t="str">
         <f t="shared" ref="T19:U19" si="20">BIN2HEX(R19,2)</f>
-        <v>00</v>
+        <v>41</v>
       </c>
       <c r="U19" s="13" t="str">
         <f t="shared" si="20"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V19" s="12">
         <v>14</v>
@@ -2270,8 +2349,8 @@
       <c r="A20" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="36" t="s">
+      <c r="B20" s="29"/>
+      <c r="C20" s="37" t="s">
         <v>64</v>
       </c>
       <c r="D20" s="17" t="s">
@@ -2346,8 +2425,8 @@
       <c r="A21" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="20" t="s">
         <v>43</v>
       </c>
@@ -2362,25 +2441,25 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="H21" s="37" t="s">
+      <c r="H21" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I21" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K21" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L21" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M21" s="37" t="s">
+      <c r="J21" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K21" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M21" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="N21" s="37" t="s">
+      <c r="N21" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O21" s="19" t="s">
@@ -2388,15 +2467,15 @@
       </c>
       <c r="P21" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>1081</v>
+        <v>10C1</v>
       </c>
       <c r="Q21" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0001000010000001</v>
+        <v>0001000011000001</v>
       </c>
       <c r="R21" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>10000001</v>
+        <v>11000001</v>
       </c>
       <c r="S21" s="12" t="str">
         <f t="shared" si="4"/>
@@ -2404,7 +2483,7 @@
       </c>
       <c r="T21" s="12" t="str">
         <f t="shared" ref="T21:U21" si="22">BIN2HEX(R21,2)</f>
-        <v>81</v>
+        <v>C1</v>
       </c>
       <c r="U21" s="13" t="str">
         <f t="shared" si="22"/>
@@ -2422,8 +2501,8 @@
       <c r="A22" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="17" t="s">
         <v>48</v>
       </c>
@@ -2436,25 +2515,25 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H22" s="37" t="s">
+      <c r="H22" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I22" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J22" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K22" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L22" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M22" s="37" t="s">
+      <c r="J22" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L22" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M22" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="N22" s="37" t="s">
+      <c r="N22" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O22" s="19" t="s">
@@ -2462,15 +2541,15 @@
       </c>
       <c r="P22" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>1101</v>
+        <v>1141</v>
       </c>
       <c r="Q22" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0001000100000001</v>
+        <v>0001000101000001</v>
       </c>
       <c r="R22" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>00000001</v>
+        <v>01000001</v>
       </c>
       <c r="S22" s="12" t="str">
         <f t="shared" si="4"/>
@@ -2478,7 +2557,7 @@
       </c>
       <c r="T22" s="12" t="str">
         <f t="shared" ref="T22:U22" si="23">BIN2HEX(R22,2)</f>
-        <v>01</v>
+        <v>41</v>
       </c>
       <c r="U22" s="13" t="str">
         <f t="shared" si="23"/>
@@ -2496,8 +2575,8 @@
       <c r="A23" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="20" t="s">
         <v>50</v>
       </c>
@@ -2510,25 +2589,25 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H23" s="37" t="s">
+      <c r="H23" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I23" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J23" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K23" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L23" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M23" s="37" t="s">
+      <c r="J23" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L23" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M23" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="N23" s="37" t="s">
+      <c r="N23" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O23" s="19" t="s">
@@ -2536,15 +2615,15 @@
       </c>
       <c r="P23" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>1201</v>
+        <v>1241</v>
       </c>
       <c r="Q23" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0001001000000001</v>
+        <v>0001001001000001</v>
       </c>
       <c r="R23" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>00000001</v>
+        <v>01000001</v>
       </c>
       <c r="S23" s="12" t="str">
         <f t="shared" si="4"/>
@@ -2552,7 +2631,7 @@
       </c>
       <c r="T23" s="12" t="str">
         <f t="shared" ref="T23:U23" si="24">BIN2HEX(R23,2)</f>
-        <v>01</v>
+        <v>41</v>
       </c>
       <c r="U23" s="13" t="str">
         <f t="shared" si="24"/>
@@ -2570,8 +2649,8 @@
       <c r="A24" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="17" t="s">
         <v>52</v>
       </c>
@@ -2586,25 +2665,25 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H24" s="37" t="s">
+      <c r="H24" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I24" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J24" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K24" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L24" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M24" s="37" t="s">
+      <c r="J24" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K24" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L24" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M24" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="N24" s="37" t="s">
+      <c r="N24" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O24" s="19" t="s">
@@ -2612,15 +2691,15 @@
       </c>
       <c r="P24" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>1281</v>
+        <v>12C1</v>
       </c>
       <c r="Q24" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0001001010000001</v>
+        <v>0001001011000001</v>
       </c>
       <c r="R24" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>10000001</v>
+        <v>11000001</v>
       </c>
       <c r="S24" s="12" t="str">
         <f t="shared" si="4"/>
@@ -2628,7 +2707,7 @@
       </c>
       <c r="T24" s="12" t="str">
         <f t="shared" ref="T24:U24" si="25">BIN2HEX(R24,2)</f>
-        <v>81</v>
+        <v>C1</v>
       </c>
       <c r="U24" s="13" t="str">
         <f t="shared" si="25"/>
@@ -2646,8 +2725,8 @@
       <c r="A25" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="17" t="s">
         <v>52</v>
       </c>
@@ -2662,25 +2741,25 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H25" s="37" t="s">
+      <c r="H25" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I25" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J25" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K25" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L25" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M25" s="37" t="s">
+      <c r="J25" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K25" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L25" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M25" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="N25" s="37" t="s">
+      <c r="N25" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O25" s="19" t="s">
@@ -2688,15 +2767,15 @@
       </c>
       <c r="P25" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>1681</v>
+        <v>16C1</v>
       </c>
       <c r="Q25" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0001011010000001</v>
+        <v>0001011011000001</v>
       </c>
       <c r="R25" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>10000001</v>
+        <v>11000001</v>
       </c>
       <c r="S25" s="12" t="str">
         <f t="shared" si="4"/>
@@ -2704,7 +2783,7 @@
       </c>
       <c r="T25" s="12" t="str">
         <f t="shared" ref="T25:U25" si="26">BIN2HEX(R25,2)</f>
-        <v>81</v>
+        <v>C1</v>
       </c>
       <c r="U25" s="13" t="str">
         <f t="shared" si="26"/>
@@ -2722,8 +2801,8 @@
       <c r="A26" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="17" t="s">
         <v>55</v>
       </c>
@@ -2736,25 +2815,25 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="H26" s="37" t="s">
+      <c r="H26" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I26" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J26" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K26" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L26" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M26" s="37" t="s">
+      <c r="J26" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K26" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L26" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M26" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="N26" s="37" t="s">
+      <c r="N26" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O26" s="19" t="s">
@@ -2762,15 +2841,15 @@
       </c>
       <c r="P26" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>1301</v>
+        <v>1341</v>
       </c>
       <c r="Q26" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0001001100000001</v>
+        <v>0001001101000001</v>
       </c>
       <c r="R26" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>00000001</v>
+        <v>01000001</v>
       </c>
       <c r="S26" s="12" t="str">
         <f t="shared" si="4"/>
@@ -2778,7 +2857,7 @@
       </c>
       <c r="T26" s="12" t="str">
         <f t="shared" ref="T26:U26" si="27">BIN2HEX(R26,2)</f>
-        <v>01</v>
+        <v>41</v>
       </c>
       <c r="U26" s="13" t="str">
         <f t="shared" si="27"/>
@@ -2796,8 +2875,8 @@
       <c r="A27" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
@@ -2810,25 +2889,25 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="H27" s="37" t="s">
+      <c r="H27" s="27" t="s">
         <v>65</v>
       </c>
       <c r="I27" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J27" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K27" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L27" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M27" s="37" t="s">
+      <c r="J27" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L27" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M27" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="N27" s="37" t="s">
+      <c r="N27" s="27" t="s">
         <v>67</v>
       </c>
       <c r="O27" s="19" t="s">
@@ -2836,15 +2915,15 @@
       </c>
       <c r="P27" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>1381</v>
+        <v>13C1</v>
       </c>
       <c r="Q27" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0001001110000001</v>
+        <v>0001001111000001</v>
       </c>
       <c r="R27" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>10000001</v>
+        <v>11000001</v>
       </c>
       <c r="S27" s="12" t="str">
         <f t="shared" si="4"/>
@@ -2852,7 +2931,7 @@
       </c>
       <c r="T27" s="12" t="str">
         <f t="shared" ref="T27:U27" si="28">BIN2HEX(R27,2)</f>
-        <v>81</v>
+        <v>C1</v>
       </c>
       <c r="U27" s="13" t="str">
         <f t="shared" si="28"/>
@@ -2870,10 +2949,10 @@
       <c r="A28" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="37" t="s">
         <v>79</v>
       </c>
       <c r="D28" s="17" t="s">
@@ -2888,37 +2967,53 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
+      <c r="H28" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="J28" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K28" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L28" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M28" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N28" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="O28" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P28" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0842</v>
       </c>
       <c r="Q28" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100001000010</v>
       </c>
       <c r="R28" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000010</v>
       </c>
       <c r="S28" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T28" s="12" t="str">
         <f t="shared" ref="T28:U28" si="29">BIN2HEX(R28,2)</f>
-        <v>00</v>
+        <v>42</v>
       </c>
       <c r="U28" s="13" t="str">
         <f t="shared" si="29"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V28" s="12">
         <v>23</v>
@@ -2928,12 +3023,12 @@
         <v>010111</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="20" t="s">
         <v>43</v>
       </c>
@@ -2946,37 +3041,53 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
+      <c r="H29" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K29" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L29" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M29" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N29" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="O29" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P29" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0842</v>
       </c>
       <c r="Q29" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100001000010</v>
       </c>
       <c r="R29" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000010</v>
       </c>
       <c r="S29" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T29" s="12" t="str">
         <f t="shared" ref="T29:U29" si="30">BIN2HEX(R29,2)</f>
-        <v>00</v>
+        <v>42</v>
       </c>
       <c r="U29" s="13" t="str">
         <f t="shared" si="30"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V29" s="12">
         <v>24</v>
@@ -2986,12 +3097,12 @@
         <v>011000</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="17" t="s">
         <v>48</v>
       </c>
@@ -3004,37 +3115,53 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
+      <c r="H30" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="J30" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K30" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L30" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M30" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N30" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="O30" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P30" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0842</v>
       </c>
       <c r="Q30" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100001000010</v>
       </c>
       <c r="R30" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000010</v>
       </c>
       <c r="S30" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T30" s="12" t="str">
         <f t="shared" ref="T30:U30" si="31">BIN2HEX(R30,2)</f>
-        <v>00</v>
+        <v>42</v>
       </c>
       <c r="U30" s="13" t="str">
         <f t="shared" si="31"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V30" s="12">
         <v>25</v>
@@ -3044,14 +3171,14 @@
         <v>011001</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="37" t="s">
         <v>84</v>
       </c>
       <c r="D31" s="17" t="s">
@@ -3066,33 +3193,49 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
+      <c r="H31" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K31" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="L31" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M31" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N31" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="O31" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P31" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0064</v>
       </c>
       <c r="Q31" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000001100100</v>
       </c>
       <c r="R31" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01100100</v>
       </c>
       <c r="S31" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T31" s="12" t="str">
         <f t="shared" ref="T31:U31" si="32">BIN2HEX(R31,2)</f>
-        <v>00</v>
+        <v>64</v>
       </c>
       <c r="U31" s="13" t="str">
         <f t="shared" si="32"/>
@@ -3106,12 +3249,12 @@
         <v>011010</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
       <c r="D32" s="20" t="s">
         <v>43</v>
       </c>
@@ -3124,33 +3267,49 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
+      <c r="H32" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K32" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="L32" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M32" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N32" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="O32" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P32" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0064</v>
       </c>
       <c r="Q32" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000001100100</v>
       </c>
       <c r="R32" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01100100</v>
       </c>
       <c r="S32" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T32" s="12" t="str">
         <f t="shared" ref="T32:U32" si="33">BIN2HEX(R32,2)</f>
-        <v>00</v>
+        <v>64</v>
       </c>
       <c r="U32" s="13" t="str">
         <f t="shared" si="33"/>
@@ -3164,12 +3323,12 @@
         <v>011011</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
       <c r="D33" s="20" t="s">
         <v>50</v>
       </c>
@@ -3182,33 +3341,49 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
+      <c r="H33" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I33" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K33" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="L33" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M33" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N33" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="O33" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P33" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0064</v>
       </c>
       <c r="Q33" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000001100100</v>
       </c>
       <c r="R33" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01100100</v>
       </c>
       <c r="S33" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T33" s="12" t="str">
         <f t="shared" ref="T33:U33" si="34">BIN2HEX(R33,2)</f>
-        <v>00</v>
+        <v>64</v>
       </c>
       <c r="U33" s="13" t="str">
         <f t="shared" si="34"/>
@@ -3222,12 +3397,12 @@
         <v>011100</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
       <c r="D34" s="17" t="s">
         <v>52</v>
       </c>
@@ -3240,33 +3415,49 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
+      <c r="H34" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I34" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="J34" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K34" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="L34" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M34" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N34" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="O34" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P34" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0064</v>
       </c>
       <c r="Q34" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000001100100</v>
       </c>
       <c r="R34" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01100100</v>
       </c>
       <c r="S34" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T34" s="12" t="str">
         <f t="shared" ref="T34:U34" si="35">BIN2HEX(R34,2)</f>
-        <v>00</v>
+        <v>64</v>
       </c>
       <c r="U34" s="13" t="str">
         <f t="shared" si="35"/>
@@ -3280,12 +3471,12 @@
         <v>011101</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="17" t="s">
         <v>55</v>
       </c>
@@ -3298,33 +3489,49 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
+      <c r="H35" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I35" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="J35" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="K35" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="L35" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M35" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N35" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="O35" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P35" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0074</v>
       </c>
       <c r="Q35" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000001110100</v>
       </c>
       <c r="R35" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01110100</v>
       </c>
       <c r="S35" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T35" s="12" t="str">
         <f t="shared" ref="T35:U35" si="36">BIN2HEX(R35,2)</f>
-        <v>00</v>
+        <v>74</v>
       </c>
       <c r="U35" s="13" t="str">
         <f t="shared" si="36"/>
@@ -3338,12 +3545,12 @@
         <v>011110</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
       <c r="D36" s="17" t="s">
         <v>57</v>
       </c>
@@ -3356,33 +3563,49 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
+      <c r="H36" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I36" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="J36" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="K36" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="L36" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M36" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N36" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="O36" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="P36" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0074</v>
       </c>
       <c r="Q36" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000001110100</v>
       </c>
       <c r="R36" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01110100</v>
       </c>
       <c r="S36" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T36" s="12" t="str">
         <f t="shared" ref="T36:U36" si="37">BIN2HEX(R36,2)</f>
-        <v>00</v>
+        <v>74</v>
       </c>
       <c r="U36" s="13" t="str">
         <f t="shared" si="37"/>
@@ -3396,11 +3619,11 @@
         <v>011111</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="36" t="s">
         <v>91</v>
       </c>
       <c r="C37" s="25" t="s">
@@ -3416,37 +3639,53 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
+      <c r="H37" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I37" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="J37" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K37" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="L37" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M37" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N37" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="O37" s="27" t="s">
+        <v>69</v>
+      </c>
       <c r="P37" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1067</v>
       </c>
       <c r="Q37" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001000001100111</v>
       </c>
       <c r="R37" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01100111</v>
       </c>
       <c r="S37" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010000</v>
       </c>
       <c r="T37" s="12" t="str">
         <f t="shared" ref="T37:U37" si="38">BIN2HEX(R37,2)</f>
-        <v>00</v>
+        <v>67</v>
       </c>
       <c r="U37" s="13" t="str">
         <f t="shared" si="38"/>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="V37" s="12">
         <v>32</v>
@@ -3456,11 +3695,11 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="28"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="25" t="s">
         <v>94</v>
       </c>
@@ -3474,37 +3713,53 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
+      <c r="H38" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="J38" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K38" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L38" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M38" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="N38" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="O38" s="27" t="s">
+        <v>69</v>
+      </c>
       <c r="P38" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>17C7</v>
       </c>
       <c r="Q38" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001011111000111</v>
       </c>
       <c r="R38" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>11000111</v>
       </c>
       <c r="S38" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010111</v>
       </c>
       <c r="T38" s="12" t="str">
         <f t="shared" ref="T38:U38" si="39">BIN2HEX(R38,2)</f>
-        <v>00</v>
+        <v>C7</v>
       </c>
       <c r="U38" s="13" t="str">
         <f t="shared" si="39"/>
-        <v>00</v>
+        <v>17</v>
       </c>
       <c r="V38" s="12">
         <v>33</v>
@@ -3514,7 +3769,7 @@
         <v>100001</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
         <v>95</v>
       </c>
@@ -3534,37 +3789,53 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
+      <c r="H39" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="J39" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K39" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="L39" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M39" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N39" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="O39" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P39" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>2069</v>
       </c>
       <c r="Q39" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0010000001101001</v>
       </c>
       <c r="R39" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01101001</v>
       </c>
       <c r="S39" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00100000</v>
       </c>
       <c r="T39" s="12" t="str">
         <f t="shared" ref="T39:U39" si="40">BIN2HEX(R39,2)</f>
-        <v>00</v>
+        <v>69</v>
       </c>
       <c r="U39" s="13" t="str">
         <f t="shared" si="40"/>
-        <v>00</v>
+        <v>20</v>
       </c>
       <c r="V39" s="12">
         <v>34</v>
@@ -3574,7 +3845,7 @@
         <v>100010</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" ht="14" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
         <v>98</v>
       </c>
@@ -3596,37 +3867,53 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
+      <c r="H40" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J40" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K40" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="L40" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M40" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N40" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="O40" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P40" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>2061</v>
       </c>
       <c r="Q40" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0010000001100001</v>
       </c>
       <c r="R40" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01100001</v>
       </c>
       <c r="S40" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00100000</v>
       </c>
       <c r="T40" s="12" t="str">
         <f t="shared" ref="T40:U40" si="41">BIN2HEX(R40,2)</f>
-        <v>00</v>
+        <v>61</v>
       </c>
       <c r="U40" s="13" t="str">
         <f t="shared" si="41"/>
-        <v>00</v>
+        <v>20</v>
       </c>
       <c r="V40" s="12">
         <v>35</v>

</xml_diff>